<commit_message>
16th may 2025- updated
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other_Notes\Python\Workspace\1stFebPythonSelenium_Framework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AACA98-22BB-46C2-B3D4-207BEE5297D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E76892-6855-4913-B7C6-373BC6EEECD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>abc1</t>
   </si>
@@ -58,19 +58,37 @@
   </si>
   <si>
     <t>Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>29.99</t>
+  </si>
+  <si>
+    <t>129.94</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>55</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF132322"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,8 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,15 +466,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2A3D38-43A1-489A-8DF4-7E698074806E}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -467,8 +487,29 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
17th may 2025- updated
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other_Notes\Python\Workspace\1stFebPythonSelenium_Framework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E76892-6855-4913-B7C6-373BC6EEECD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982BAE95-F6E9-46B2-A1E0-0C65368DAB00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>